<commit_message>
chopped end years off data, gave 'province' a column name
</commit_message>
<xml_diff>
--- a/Data/fishing_fish3_province.xlsx
+++ b/Data/fishing_fish3_province.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Iwen\SFG\China\China Data Spreadsheets (by data)\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10122" windowHeight="5166" firstSheet="30" activeTab="36"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10125" windowHeight="5160" tabRatio="885" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="38" r:id="rId1"/>
@@ -25,37 +20,13 @@
     <sheet name="2005" sheetId="4" r:id="rId11"/>
     <sheet name="2004" sheetId="5" r:id="rId12"/>
     <sheet name="2003" sheetId="6" r:id="rId13"/>
-    <sheet name="2002" sheetId="7" r:id="rId14"/>
-    <sheet name="2001" sheetId="8" r:id="rId15"/>
-    <sheet name="2000" sheetId="10" r:id="rId16"/>
-    <sheet name="1999" sheetId="11" r:id="rId17"/>
-    <sheet name="1998" sheetId="12" r:id="rId18"/>
-    <sheet name="1997" sheetId="13" r:id="rId19"/>
-    <sheet name="1996" sheetId="14" r:id="rId20"/>
-    <sheet name="1995" sheetId="15" r:id="rId21"/>
-    <sheet name="1994" sheetId="16" r:id="rId22"/>
-    <sheet name="1993" sheetId="17" r:id="rId23"/>
-    <sheet name="1992" sheetId="18" r:id="rId24"/>
-    <sheet name="1991" sheetId="19" r:id="rId25"/>
-    <sheet name="1990" sheetId="20" r:id="rId26"/>
-    <sheet name="1989" sheetId="21" r:id="rId27"/>
-    <sheet name="1988" sheetId="22" r:id="rId28"/>
-    <sheet name="1987" sheetId="23" r:id="rId29"/>
-    <sheet name="1986" sheetId="24" r:id="rId30"/>
-    <sheet name="1985" sheetId="25" r:id="rId31"/>
-    <sheet name="1984" sheetId="26" r:id="rId32"/>
-    <sheet name="1983" sheetId="27" r:id="rId33"/>
-    <sheet name="1982" sheetId="28" r:id="rId34"/>
-    <sheet name="1981" sheetId="29" r:id="rId35"/>
-    <sheet name="1980" sheetId="30" r:id="rId36"/>
-    <sheet name="1979" sheetId="31" r:id="rId37"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="459">
   <si>
     <t/>
   </si>
@@ -1429,6 +1400,9 @@
   </si>
   <si>
     <t>largehead hairtail</t>
+  </si>
+  <si>
+    <t>Province</t>
   </si>
 </sst>
 </file>
@@ -1464,17 +1438,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1747,7 +1713,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1757,13 +1723,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>454</v>
       </c>
@@ -1804,7 +1773,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1821,7 +1790,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1853,7 +1822,7 @@
         <v>6606</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1894,7 +1863,7 @@
         <v>9262</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1920,7 +1889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1955,7 +1924,7 @@
         <v>11682</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1999,7 +1968,7 @@
         <v>30452</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2043,7 +2012,7 @@
         <v>22631</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2078,7 +2047,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2122,7 +2091,7 @@
         <v>23415</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2157,7 +2126,7 @@
         <v>8504</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2210,13 +2179,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>450</v>
       </c>
@@ -2245,7 +2217,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2277,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2309,7 +2281,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2341,7 +2313,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2373,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2405,7 +2377,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2437,7 +2409,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2469,7 +2441,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2501,7 +2473,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2533,7 +2505,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2565,7 +2537,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2597,7 +2569,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -2638,11 +2610,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>449</v>
       </c>
@@ -2668,7 +2645,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2697,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2726,7 +2703,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2755,7 +2732,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2784,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2813,7 +2790,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2842,7 +2819,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2871,7 +2848,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2900,7 +2877,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2929,7 +2906,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2958,7 +2935,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2987,7 +2964,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -3025,13 +3002,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>451</v>
       </c>
@@ -3054,7 +3034,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3080,7 +3060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3106,7 +3086,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3132,7 +3112,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3158,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3184,7 +3164,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3210,7 +3190,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3236,7 +3216,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3262,7 +3242,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3288,7 +3268,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3314,7 +3294,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3340,7 +3320,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>306</v>
       </c>
@@ -3375,15 +3355,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>458</v>
       </c>
       <c r="B1" t="s">
         <v>451</v>
@@ -3407,7 +3387,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3433,7 +3413,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3459,7 +3439,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3485,7 +3465,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3511,7 +3491,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3537,7 +3517,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3563,7 +3543,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3589,7 +3569,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3615,7 +3595,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3641,7 +3621,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3667,7 +3647,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3693,7 +3673,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>306</v>
       </c>
@@ -3718,216 +3698,6 @@
       <c r="H13" t="s">
         <v>453</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:P16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F2:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="15.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.47265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.15625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.41796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.89453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.47265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="1" width="11.9453125" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F2:G12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="6" max="6" width="7.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.9453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F8" s="5"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F10" s="5"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F11" s="5"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F12" s="5"/>
-      <c r="G12" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F7:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="6" max="6" width="13.9453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.9453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="6:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3938,13 +3708,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>454</v>
       </c>
@@ -3970,7 +3743,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3980,14 +3753,14 @@
       <c r="G2">
         <v>288</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="1">
         <v>6031</v>
       </c>
       <c r="I2">
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3997,49 +3770,49 @@
       <c r="D3">
         <v>123</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>6240</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>10943</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="1">
         <v>1644</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>13206</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>6618</v>
       </c>
       <c r="C4">
         <v>170</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>6837</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <v>13275</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="1">
         <v>115</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>23461</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="1">
         <v>34194</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>70156</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4049,376 +3822,202 @@
       <c r="E5">
         <v>379</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="1">
         <v>5</v>
       </c>
       <c r="I5">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>73486</v>
       </c>
       <c r="C6">
         <v>216</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>1120</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>54176</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>9218</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>5900</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="1">
         <v>8378</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>188497</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>15306</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>31344</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>414978</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>5241</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>7000</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>176293</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>71266</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>22344</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>4693</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>19904</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>180086</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>10076</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>14550</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>126798</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>52072</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>600</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>39948</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>69506</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>33729</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="1">
         <v>69555</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="1">
         <v>176471</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>3631</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>9104</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>1560</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>152279</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="1">
         <v>87532</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>25654</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="1">
         <v>31603</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <v>27914</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
         <v>42</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>31318</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="1">
         <v>35474</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>10531</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="1">
         <v>13633</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="1">
         <v>2234</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>3279</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>12619</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>16202</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="1">
         <v>161375</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>272825</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>19489</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="1">
         <v>14769</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="1">
         <v>61915</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="4"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:S35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:S34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4427,13 +4026,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>454</v>
       </c>
@@ -4459,7 +4061,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4469,14 +4071,14 @@
       <c r="G2">
         <v>195</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="1">
         <v>3970</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="1">
         <v>1697</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4486,49 +4088,49 @@
       <c r="D3">
         <v>150</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>5745</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>12534</v>
       </c>
       <c r="H3">
         <v>72</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>15912</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>7770</v>
       </c>
       <c r="C4">
         <v>200</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>7896</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <v>17113</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="1">
         <v>121</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>22542</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="1">
         <v>54403</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>83369</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4545,302 +4147,192 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>75245</v>
       </c>
       <c r="C6">
         <v>216</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>1158</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>56673</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>8357</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>8835</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="1">
         <v>8735</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>169131</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>15673</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>28113</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>440483</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>3958</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>7428</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>183371</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>71630</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>21733</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>4950</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>20225</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>166897</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>10482</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>14505</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>123429</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>50039</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>60209</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>90415</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>33618</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="1">
         <v>82960</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="1">
         <v>173653</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>2579</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>8141</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>1421</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>141228</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="1">
         <v>83193</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>22459</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="1">
         <v>29980</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <v>27712</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="C11">
         <v>40</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>30971</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="1">
         <v>35344</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>10433</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="1">
         <v>13621</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="1">
         <v>2200</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>1470</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>13411</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>1047</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="1">
         <v>146754</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>198557</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>10247</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="1">
         <v>10857</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="1">
         <v>36985</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:R34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4849,13 +4341,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>454</v>
       </c>
@@ -4881,7 +4376,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4894,14 +4389,14 @@
       <c r="G2">
         <v>305</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="1">
         <v>1440</v>
       </c>
       <c r="I2">
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4911,49 +4406,49 @@
       <c r="D3">
         <v>67</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>5740</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="1">
         <v>8425</v>
       </c>
       <c r="H3">
         <v>58</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="1">
         <v>13101</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>7979</v>
       </c>
       <c r="C4">
         <v>500</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>9054</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <v>21846</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="1">
         <v>125</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>23107</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="1">
         <v>37982</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>75522</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4970,191 +4465,191 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="1">
         <v>77602</v>
       </c>
       <c r="C6">
         <v>220</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>1200</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>57322</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="1">
         <v>358</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>9585</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>18819</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="1">
         <v>8324</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>178273</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>15891</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>30130</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>452498</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>3306</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>6544</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>190381</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>66979</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>21125</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>4496</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>19760</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>165420</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>10444</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>16307</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>120776</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>51943</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>985</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>72361</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>82402</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>32251</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="1">
         <v>85480</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="1">
         <v>174569</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>2747</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>9195</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>1437</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>133344</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="1">
         <v>84418</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>22307</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="1">
         <v>30175</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <v>29469</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>31424</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="1">
         <v>36241</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>10497</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="1">
         <v>13680</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="1">
         <v>2207</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>1463</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>13322</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>1033</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="1">
         <v>146172</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>197300</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>10095</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="1">
         <v>10753</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="1">
         <v>36805</v>
       </c>
     </row>
@@ -5167,95 +4662,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
         <v>235</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="1">
         <v>2147</v>
       </c>
       <c r="E2">
         <v>348</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
         <v>8918</v>
       </c>
       <c r="D3">
         <v>55</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="1">
         <v>5343</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
         <v>1991</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="1">
         <v>2940</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>120</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <v>26048</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>44980</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="1">
         <v>75272</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <v>5674</v>
       </c>
       <c r="H4">
@@ -5264,11 +4762,11 @@
       <c r="I4">
         <v>50</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="1">
         <v>13388</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5285,116 +4783,116 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="1">
         <v>9609</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="1">
         <v>18659</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="1">
         <v>10649</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
         <v>37667</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>2171</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="1">
         <v>13218</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="1">
         <v>2477</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="1">
         <v>7620</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="1">
         <v>231373</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="1">
         <v>68744</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="1">
         <v>7340</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>115104</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>32833</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>1615</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="1">
         <v>19648</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>10801</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="1">
         <v>17045</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="1">
         <v>127422</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="1">
         <v>50751</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="1">
         <v>3270</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="1">
         <v>60616</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="1">
         <v>60714</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>10341</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="1">
         <v>20603</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
         <v>37923</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="1">
         <v>82983</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="1">
         <v>191259</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
         <v>30727</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="1">
         <v>4042</v>
       </c>
       <c r="I9">
@@ -5404,97 +4902,97 @@
         <v>826</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>83051</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="1">
         <v>23000</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="1">
         <v>31524</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="1">
         <v>27978</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="1">
         <v>16846</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>55642</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="1">
         <v>54868</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <v>3715</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="1">
         <v>25198</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="1">
         <v>36414</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="1">
         <v>10499</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="1">
         <v>13711</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="1">
         <v>2221</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
         <v>11835</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="1">
         <v>29947</v>
       </c>
       <c r="I11">
         <v>414</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="1">
         <v>8028</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>190195</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="1">
         <v>9739</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="1">
         <v>10286</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="1">
         <v>35222</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>15890</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>39065</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="1">
         <v>17104</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="1">
         <v>13539</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="1">
         <v>12841</v>
       </c>
     </row>
@@ -5507,13 +5005,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>454</v>
       </c>
@@ -5554,7 +5055,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5577,7 +5078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5606,7 +5107,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5647,7 +5148,7 @@
         <v>5122</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -5667,7 +5168,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -5705,7 +5206,7 @@
         <v>14523</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5749,7 +5250,7 @@
         <v>12024</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -5793,7 +5294,7 @@
         <v>15811</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5834,7 +5335,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5878,7 +5379,7 @@
         <v>21462</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5916,7 +5417,7 @@
         <v>7887</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5969,13 +5470,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>454</v>
       </c>
@@ -6016,7 +5520,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6039,7 +5543,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6065,7 +5569,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6106,7 +5610,7 @@
         <v>4563</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6129,7 +5633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6164,7 +5668,7 @@
         <v>10968</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6208,7 +5712,7 @@
         <v>10677</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6252,7 +5756,7 @@
         <v>15913</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -6290,7 +5794,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6334,7 +5838,7 @@
         <v>25353</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6375,7 +5879,7 @@
         <v>8054</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -6428,18 +5932,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="13.05078125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>458</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -6457,7 +5961,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6477,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6497,7 +6001,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6517,7 +6021,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6537,7 +6041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6557,7 +6061,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6577,7 +6081,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6597,7 +6101,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -6617,7 +6121,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -6637,7 +6141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6657,7 +6161,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -6686,11 +6190,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>458</v>
+      </c>
       <c r="B1" t="s">
         <v>450</v>
       </c>
@@ -6719,7 +6228,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -6751,7 +6260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6783,7 +6292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -6815,7 +6324,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -6847,7 +6356,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -6879,7 +6388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -6911,7 +6420,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -6943,7 +6452,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -6975,7 +6484,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -7007,7 +6516,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -7039,7 +6548,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -7071,7 +6580,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -7103,7 +6612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>

</xml_diff>